<commit_message>
Maven fertig, aber error nach Login
</commit_message>
<xml_diff>
--- a/group5/src/main/resources/databases/DefaultUSERS.xlsx
+++ b/group5/src/main/resources/databases/DefaultUSERS.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="70">
   <si>
     <t>Max</t>
   </si>
@@ -717,7 +717,7 @@
         <v>1.0</v>
       </c>
       <c r="K2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Änderungen am ToDoPanel reingemacht, Auslogger bei Fensterschließen umgestellt
</commit_message>
<xml_diff>
--- a/group5/src/main/resources/databases/DefaultUSERS.xlsx
+++ b/group5/src/main/resources/databases/DefaultUSERS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\Documents\GitHub Repositories\HWG Repos\ATdIT_Gruppe5\databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\Documents\GitHub Repositories\HWG Repos\ATdIT_Gruppe5\group5\src\main\resources\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D5173E-A830-467E-84C8-1F4801C2E64F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8C5D0F-5861-4AAE-84B1-5A7C86D9D197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>Max</t>
   </si>
@@ -233,19 +233,10 @@
     <t>test</t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>passwort1234</t>
-  </si>
-  <si>
-    <t>.Test</t>
-  </si>
-  <si>
-    <t>Test</t>
+    <t/>
+  </si>
+  <si>
+    <t>..._...@....</t>
   </si>
 </sst>
 </file>
@@ -634,7 +625,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,13 +696,13 @@
         <v>66</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>11111.0</v>
+        <v>0.0</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>66</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>65</v>
@@ -724,8 +715,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="n">
-        <v>1.0</v>
+      <c r="A3" s="3">
+        <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>60</v>
@@ -739,8 +730,8 @@
       <c r="E3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="3" t="n">
-        <v>12345.0</v>
+      <c r="F3" s="3">
+        <v>12345</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>63</v>
@@ -751,11 +742,11 @@
       <c r="I3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="3" t="n">
-        <v>1.0</v>
+      <c r="J3" s="3">
+        <v>1</v>
       </c>
       <c r="K3" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
alles zu private, serialVersionId angepasst
</commit_message>
<xml_diff>
--- a/group5/src/main/resources/databases/DefaultUSERS.xlsx
+++ b/group5/src/main/resources/databases/DefaultUSERS.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\Documents\GitHub Repositories\HWG Repos\ATdIT_Gruppe5\group5\src\main\resources\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8C5D0F-5861-4AAE-84B1-5A7C86D9D197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3341C8-0C84-4BC0-8D42-F6693449A147}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t>Max</t>
   </si>
@@ -233,10 +233,19 @@
     <t>test</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>..._...@....</t>
+  </si>
+  <si>
+    <t>TestVorname</t>
+  </si>
+  <si>
+    <t>TestNachname</t>
+  </si>
+  <si>
+    <t>Teststraße 0</t>
+  </si>
+  <si>
+    <t>Teststadt</t>
   </si>
 </sst>
 </file>
@@ -625,23 +634,23 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="13.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="16.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="8.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="5" width="21.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="5" width="32.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="7.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="11.28515625" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="11.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -680,35 +689,35 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="n">
-        <v>0.0</v>
+      <c r="A2" s="3">
+        <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="3" t="n">
-        <v>1.0</v>
+      <c r="J2" s="3">
+        <v>1</v>
       </c>
       <c r="K2" s="1" t="b">
         <v>0</v>

</xml_diff>